<commit_message>
Update maven dependencies and some minor changes
</commit_message>
<xml_diff>
--- a/src/test/report/TestLog.xlsx
+++ b/src/test/report/TestLog.xlsx
@@ -527,9 +527,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -542,34 +539,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <b val="0"/>
@@ -620,8 +597,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="5"/>
-      <tableStyleElement type="headerRow" dxfId="4"/>
+      <tableStyleElement type="wholeTable" dxfId="3"/>
+      <tableStyleElement type="headerRow" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -901,29 +878,29 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.7265625" style="2" customWidth="1"/>
     <col min="3" max="3" width="14.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="118.6328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="89.81640625" style="2" customWidth="1"/>
     <col min="5" max="16384" width="14.453125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>26</v>
       </c>
       <c r="E1" s="1"/>
@@ -1714,12 +1691,12 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1744,10 +1721,10 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="22"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -29020,12 +28997,12 @@
     <mergeCell ref="A26:D27"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:D24">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>$C2="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D24">
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="0" priority="5">
       <formula>$C2="Fail"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>